<commit_message>
19 Oct 2017 Final
</commit_message>
<xml_diff>
--- a/clientdata/CROP BIFURCATION.xlsx
+++ b/clientdata/CROP BIFURCATION.xlsx
@@ -1,21 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tejaswini\Desktop\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" xr2:uid="{B326D37B-027E-4B7D-8324-A5C0F23B7198}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530"/>
   </bookViews>
   <sheets>
     <sheet name="CROP VARIETY" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="261">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="247">
   <si>
     <t>CROP GROUP</t>
   </si>
@@ -165,9 +160,6 @@
     <t>Black Gram (Urd)</t>
   </si>
   <si>
-    <t>Bengal Gram (Kabuli Chana)</t>
-  </si>
-  <si>
     <t>Cowpea (Asparagus)</t>
   </si>
   <si>
@@ -207,18 +199,12 @@
     <t>Lethyrus</t>
   </si>
   <si>
-    <t>Mochai (Lab lab)</t>
-  </si>
-  <si>
     <t>OILSEEDS</t>
   </si>
   <si>
     <t>Castor</t>
   </si>
   <si>
-    <t>Groundnut</t>
-  </si>
-  <si>
     <t>Mustard (Sarso)</t>
   </si>
   <si>
@@ -315,9 +301,6 @@
     <t>Nutmeg</t>
   </si>
   <si>
-    <t>Fenugreek</t>
-  </si>
-  <si>
     <t>Mint</t>
   </si>
   <si>
@@ -426,9 +409,6 @@
     <t>Sweet Potato</t>
   </si>
   <si>
-    <t>Carrot</t>
-  </si>
-  <si>
     <t>Radish</t>
   </si>
   <si>
@@ -447,12 +427,6 @@
     <t>GREEN LEAFY VEGETABLES</t>
   </si>
   <si>
-    <t>Amaranthus</t>
-  </si>
-  <si>
-    <t>Spinach</t>
-  </si>
-  <si>
     <t>Lettuce</t>
   </si>
   <si>
@@ -462,18 +436,9 @@
     <t>Capsicum</t>
   </si>
   <si>
-    <t>Brinjal</t>
-  </si>
-  <si>
-    <t>Chillies</t>
-  </si>
-  <si>
     <t>Lady Finger</t>
   </si>
   <si>
-    <t>Tomato</t>
-  </si>
-  <si>
     <t>FRUIT CROPS</t>
   </si>
   <si>
@@ -486,12 +451,6 @@
     <t>CUCURBITS</t>
   </si>
   <si>
-    <t>Bitter Gourd</t>
-  </si>
-  <si>
-    <t>Bottle Gourd</t>
-  </si>
-  <si>
     <t>Pumpkin</t>
   </si>
   <si>
@@ -504,9 +463,6 @@
     <t>Long Melon</t>
   </si>
   <si>
-    <t>Ridge Gourd</t>
-  </si>
-  <si>
     <t>Pointed Gourd (Parwal)</t>
   </si>
   <si>
@@ -565,9 +521,6 @@
   </si>
   <si>
     <t>Garlic</t>
-  </si>
-  <si>
-    <t>Onion</t>
   </si>
   <si>
     <t>FORAGE CROPS</t>
@@ -813,7 +766,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -960,7 +913,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -1012,7 +965,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -1206,25 +1159,26 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B953106-9DBB-4C38-AD30-EDCCBF2518E7}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D235"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.140625" style="3" customWidth="1"/>
+    <col min="1" max="1" width="24.140625" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21.7109375" style="3" customWidth="1"/>
-    <col min="3" max="4" width="9.140625" style="4"/>
+    <col min="3" max="3" width="12.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -1458,1053 +1412,982 @@
         <v>45</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B37" s="3" t="s">
-        <v>46</v>
-      </c>
-    </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B38" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B39" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B40" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B41" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B42" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B43" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B44" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B45" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B46" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B47" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B48" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B49" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B50" s="3" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B51" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B53" s="3" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B54" s="3" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B55" s="3" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B56" s="3" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B57" s="3" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B58" s="3" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B59" s="3" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B60" s="3" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B61" s="3" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B62" s="3" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B63" s="3" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B64" s="3" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B65" s="3" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B66" s="3" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B67" s="3" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" s="3" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B69" s="3" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B70" s="3" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B71" s="3" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B72" s="3" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" s="3" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B74" s="3" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B75" s="3" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" s="3" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B77" s="3" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B78" s="3" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B79" s="3" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B80" s="3" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="81" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B81" s="3" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="82" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B82" s="3" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="83" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B83" s="3" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
     </row>
     <row r="84" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B84" s="3" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
     </row>
     <row r="85" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B85" s="3" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="86" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B86" s="3" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
     <row r="87" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B87" s="3" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
     </row>
     <row r="88" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B88" s="3" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
     </row>
     <row r="89" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B89" s="3" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
     </row>
     <row r="90" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B90" s="3" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="91" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B91" s="3" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="92" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B92" s="3" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="93" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B93" s="3" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
     </row>
     <row r="94" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B94" s="3" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
     <row r="95" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B95" s="3" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="96" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B96" s="3" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B97" s="3" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B98" s="3" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B99" s="3" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B100" s="3" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B101" s="3" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B102" s="3" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" s="3" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="B103" s="3" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B104" s="3" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B105" s="3" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B106" s="3" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B107" s="3" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B108" s="3" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" s="3" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="B109" s="3" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B110" s="3" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B111" s="3" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B112" s="3" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B113" s="3" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B114" s="3" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B115" s="3" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" s="3" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="B116" s="3" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B117" s="3" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B118" s="3" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B119" s="3" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B120" s="3" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121" s="3" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="B121" s="3" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="B122" s="3" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B123" s="3" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B124" s="3" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B125" s="3" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126" s="3" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="B126" s="3" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B127" s="3" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B128" s="3" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B129" s="3" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B130" s="3" t="s">
-        <v>148</v>
+        <v>138</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A131" s="3" t="s">
-        <v>149</v>
+        <v>139</v>
       </c>
       <c r="B131" s="3" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B132" s="3" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B133" s="3" t="s">
-        <v>158</v>
+        <v>146</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B134" s="3" t="s">
-        <v>168</v>
+        <v>155</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B135" s="3" t="s">
-        <v>199</v>
+        <v>185</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B136" s="3" t="s">
-        <v>200</v>
+        <v>186</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B137" s="3" t="s">
-        <v>201</v>
+        <v>187</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B138" s="3" t="s">
-        <v>202</v>
+        <v>188</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B139" s="3" t="s">
-        <v>203</v>
+        <v>189</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B140" s="3" t="s">
-        <v>204</v>
+        <v>190</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B141" s="3" t="s">
-        <v>205</v>
+        <v>191</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B142" s="3" t="s">
-        <v>206</v>
+        <v>192</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B143" s="3" t="s">
-        <v>207</v>
+        <v>193</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B144" s="3" t="s">
-        <v>208</v>
+        <v>194</v>
       </c>
     </row>
     <row r="145" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B145" s="3" t="s">
-        <v>209</v>
+        <v>195</v>
       </c>
     </row>
     <row r="146" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B146" s="3" t="s">
-        <v>210</v>
+        <v>196</v>
       </c>
     </row>
     <row r="147" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B147" s="3" t="s">
-        <v>211</v>
+        <v>197</v>
       </c>
     </row>
     <row r="148" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B148" s="3" t="s">
-        <v>212</v>
+        <v>198</v>
       </c>
     </row>
     <row r="149" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B149" s="3" t="s">
-        <v>213</v>
+        <v>199</v>
       </c>
     </row>
     <row r="150" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B150" s="3" t="s">
-        <v>214</v>
+        <v>200</v>
       </c>
     </row>
     <row r="151" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B151" s="3" t="s">
-        <v>215</v>
+        <v>201</v>
       </c>
     </row>
     <row r="152" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B152" s="3" t="s">
-        <v>216</v>
+        <v>202</v>
       </c>
     </row>
     <row r="153" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B153" s="3" t="s">
-        <v>217</v>
+        <v>203</v>
       </c>
     </row>
     <row r="154" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B154" s="3" t="s">
-        <v>218</v>
+        <v>204</v>
       </c>
     </row>
     <row r="155" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B155" s="3" t="s">
-        <v>219</v>
+        <v>205</v>
       </c>
     </row>
     <row r="156" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B156" s="3" t="s">
-        <v>247</v>
+        <v>233</v>
       </c>
     </row>
     <row r="157" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B157" s="3" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
     </row>
     <row r="158" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B158" s="3" t="s">
-        <v>248</v>
+        <v>234</v>
       </c>
     </row>
     <row r="159" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B159" s="3" t="s">
-        <v>221</v>
+        <v>207</v>
       </c>
     </row>
     <row r="160" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B160" s="3" t="s">
-        <v>222</v>
+        <v>208</v>
       </c>
     </row>
     <row r="161" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B161" s="3" t="s">
-        <v>151</v>
+        <v>141</v>
       </c>
     </row>
     <row r="162" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B162" s="3" t="s">
-        <v>223</v>
+        <v>209</v>
       </c>
     </row>
     <row r="163" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B163" s="3" t="s">
-        <v>224</v>
+        <v>210</v>
       </c>
     </row>
     <row r="164" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B164" s="3" t="s">
-        <v>245</v>
+        <v>231</v>
       </c>
     </row>
     <row r="165" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B165" s="3" t="s">
-        <v>246</v>
+        <v>232</v>
       </c>
     </row>
     <row r="166" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B166" s="3" t="s">
-        <v>225</v>
+        <v>211</v>
       </c>
     </row>
     <row r="167" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B167" s="3" t="s">
-        <v>226</v>
+        <v>212</v>
       </c>
     </row>
     <row r="168" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B168" s="3" t="s">
-        <v>227</v>
+        <v>213</v>
       </c>
     </row>
     <row r="169" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B169" s="3" t="s">
-        <v>228</v>
+        <v>214</v>
       </c>
     </row>
     <row r="170" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B170" s="3" t="s">
-        <v>229</v>
+        <v>215</v>
       </c>
     </row>
     <row r="171" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B171" s="3" t="s">
-        <v>230</v>
+        <v>216</v>
       </c>
     </row>
     <row r="172" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B172" s="3" t="s">
-        <v>231</v>
+        <v>217</v>
       </c>
     </row>
     <row r="173" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B173" s="3" t="s">
-        <v>232</v>
+        <v>218</v>
       </c>
     </row>
     <row r="174" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B174" s="3" t="s">
-        <v>233</v>
+        <v>219</v>
       </c>
     </row>
     <row r="175" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B175" s="3" t="s">
-        <v>234</v>
+        <v>220</v>
       </c>
     </row>
     <row r="176" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B176" s="3" t="s">
-        <v>169</v>
+        <v>156</v>
       </c>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B177" s="3" t="s">
-        <v>151</v>
+        <v>141</v>
       </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A178" s="3" t="s">
-        <v>152</v>
-      </c>
-      <c r="B178" s="3" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="179" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B179" s="3" t="s">
-        <v>154</v>
+        <v>142</v>
       </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B180" s="3" t="s">
-        <v>155</v>
+        <v>143</v>
       </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B181" s="3" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="182" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B182" s="3" t="s">
-        <v>159</v>
+        <v>144</v>
       </c>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B183" s="3" t="s">
-        <v>160</v>
+        <v>147</v>
       </c>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B184" s="3" t="s">
-        <v>161</v>
+        <v>148</v>
       </c>
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B185" s="3" t="s">
-        <v>162</v>
+        <v>149</v>
       </c>
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B186" s="3" t="s">
-        <v>163</v>
+        <v>150</v>
       </c>
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B187" s="3" t="s">
-        <v>164</v>
+        <v>151</v>
       </c>
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B188" s="3" t="s">
-        <v>165</v>
+        <v>152</v>
       </c>
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B189" s="3" t="s">
-        <v>166</v>
+        <v>153</v>
       </c>
     </row>
     <row r="190" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B190" s="3" t="s">
-        <v>167</v>
+        <v>154</v>
       </c>
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A191" s="3" t="s">
-        <v>170</v>
+        <v>157</v>
       </c>
       <c r="B191" s="3" t="s">
-        <v>171</v>
+        <v>158</v>
       </c>
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B192" s="3" t="s">
-        <v>172</v>
+        <v>159</v>
       </c>
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B193" s="3" t="s">
-        <v>173</v>
+        <v>160</v>
       </c>
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B194" s="3" t="s">
-        <v>174</v>
+        <v>161</v>
       </c>
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A195" s="3" t="s">
-        <v>175</v>
+        <v>162</v>
       </c>
       <c r="B195" s="3" t="s">
-        <v>176</v>
+        <v>163</v>
       </c>
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B196" s="3" t="s">
-        <v>177</v>
+        <v>164</v>
       </c>
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A197" s="3" t="s">
-        <v>178</v>
+        <v>165</v>
       </c>
       <c r="B197" s="3" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="198" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B198" s="3" t="s">
-        <v>180</v>
+        <v>166</v>
       </c>
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A199" s="3" t="s">
-        <v>181</v>
+        <v>167</v>
       </c>
       <c r="B199" s="3" t="s">
-        <v>182</v>
+        <v>168</v>
       </c>
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B200" s="3" t="s">
-        <v>183</v>
+        <v>169</v>
       </c>
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B201" s="3" t="s">
-        <v>184</v>
+        <v>170</v>
       </c>
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B202" s="3" t="s">
-        <v>185</v>
+        <v>171</v>
       </c>
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B203" s="3" t="s">
-        <v>186</v>
+        <v>172</v>
       </c>
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B204" s="3" t="s">
-        <v>187</v>
+        <v>173</v>
       </c>
     </row>
     <row r="205" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B205" s="3" t="s">
-        <v>188</v>
+        <v>174</v>
       </c>
     </row>
     <row r="206" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B206" s="3" t="s">
-        <v>189</v>
+        <v>175</v>
       </c>
     </row>
     <row r="207" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B207" s="3" t="s">
-        <v>190</v>
+        <v>176</v>
       </c>
     </row>
     <row r="208" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B208" s="3" t="s">
-        <v>191</v>
+        <v>177</v>
       </c>
     </row>
     <row r="209" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B209" s="3" t="s">
-        <v>192</v>
+        <v>178</v>
       </c>
     </row>
     <row r="210" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B210" s="3" t="s">
-        <v>193</v>
+        <v>179</v>
       </c>
     </row>
     <row r="211" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B211" s="3" t="s">
-        <v>194</v>
+        <v>180</v>
       </c>
     </row>
     <row r="212" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B212" s="3" t="s">
-        <v>195</v>
+        <v>181</v>
       </c>
     </row>
     <row r="213" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B213" s="3" t="s">
-        <v>196</v>
+        <v>182</v>
       </c>
     </row>
     <row r="214" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B214" s="3" t="s">
-        <v>197</v>
+        <v>183</v>
       </c>
     </row>
     <row r="215" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B215" s="3" t="s">
-        <v>198</v>
+        <v>184</v>
       </c>
     </row>
     <row r="216" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A216" s="3" t="s">
-        <v>235</v>
+        <v>221</v>
       </c>
       <c r="B216" s="3" t="s">
-        <v>236</v>
+        <v>222</v>
       </c>
     </row>
     <row r="217" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B217" s="3" t="s">
-        <v>237</v>
+        <v>223</v>
       </c>
     </row>
     <row r="218" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B218" s="3" t="s">
-        <v>238</v>
+        <v>224</v>
       </c>
     </row>
     <row r="219" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B219" s="3" t="s">
-        <v>239</v>
+        <v>225</v>
       </c>
     </row>
     <row r="220" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B220" s="3" t="s">
-        <v>240</v>
+        <v>226</v>
       </c>
     </row>
     <row r="221" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B221" s="3" t="s">
-        <v>241</v>
+        <v>227</v>
       </c>
     </row>
     <row r="222" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B222" s="3" t="s">
-        <v>242</v>
+        <v>228</v>
       </c>
     </row>
     <row r="223" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B223" s="3" t="s">
-        <v>243</v>
+        <v>229</v>
       </c>
     </row>
     <row r="224" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B224" s="3" t="s">
-        <v>244</v>
+        <v>230</v>
       </c>
     </row>
     <row r="225" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B225" s="7" t="s">
-        <v>249</v>
+        <v>235</v>
       </c>
     </row>
     <row r="226" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B226" s="7" t="s">
-        <v>250</v>
+        <v>236</v>
       </c>
     </row>
     <row r="227" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B227" s="7" t="s">
-        <v>251</v>
+        <v>237</v>
       </c>
     </row>
     <row r="228" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B228" s="7" t="s">
-        <v>252</v>
+        <v>238</v>
       </c>
     </row>
     <row r="229" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B229" s="8" t="s">
-        <v>253</v>
+        <v>239</v>
       </c>
     </row>
     <row r="230" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B230" s="8" t="s">
-        <v>254</v>
+        <v>240</v>
       </c>
     </row>
     <row r="231" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B231" s="8" t="s">
-        <v>255</v>
+        <v>241</v>
       </c>
     </row>
     <row r="232" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B232" s="8" t="s">
-        <v>256</v>
+        <v>242</v>
       </c>
     </row>
     <row r="233" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A233" s="3" t="s">
-        <v>257</v>
+        <v>243</v>
       </c>
       <c r="B233" s="3" t="s">
-        <v>258</v>
+        <v>244</v>
       </c>
     </row>
     <row r="234" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B234" s="3" t="s">
-        <v>259</v>
+        <v>245</v>
       </c>
     </row>
     <row r="235" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B235" s="3" t="s">
-        <v>260</v>
+        <v>246</v>
       </c>
     </row>
   </sheetData>
@@ -2514,7 +2397,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{257AE80E-5A34-49EF-B477-F7897ACBB185}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>